<commit_message>
Vignette updated with period_fun function when reading an Excel file. Na's in files replaced by empty cells.
</commit_message>
<xml_diff>
--- a/pkg/vignettes/testlabels.xlsx
+++ b/pkg/vignettes/testlabels.xlsx
@@ -64,7 +64,7 @@
     <t>labour</t>
   </si>
   <si>
-    <t>NA</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Vignette: in section labels text added and examples updated; in section 'period and period_range' description period extended, new subsection added with functions get_periods and seq,  examples updated;
Reference manual: several typing errors updated, print removed in example cvgdif, description and examples period function updated.
</commit_message>
<xml_diff>
--- a/pkg/vignettes/testlabels.xlsx
+++ b/pkg/vignettes/testlabels.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>bbpwn</t>
-  </si>
-  <si>
     <t>label</t>
   </si>
   <si>
@@ -40,31 +37,28 @@
     <t>bbp</t>
   </si>
   <si>
-    <t>taxes</t>
-  </si>
-  <si>
-    <t>bet_wn</t>
-  </si>
-  <si>
-    <t>clt_wn</t>
-  </si>
-  <si>
-    <t>expenses</t>
-  </si>
-  <si>
-    <t>hl__hr</t>
-  </si>
-  <si>
-    <t>productivity</t>
-  </si>
-  <si>
-    <t>a__mn_</t>
-  </si>
-  <si>
-    <t>labour</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a__m_mn_ </t>
+  </si>
+  <si>
+    <t>bbp_m_wn</t>
+  </si>
+  <si>
+    <t>bet_c_wn</t>
+  </si>
+  <si>
+    <t>clt_c_wn</t>
+  </si>
+  <si>
+    <t>arbeidsvolume</t>
+  </si>
+  <si>
+    <t>belasting</t>
+  </si>
+  <si>
+    <t>coll.lasten</t>
   </si>
 </sst>
 </file>
@@ -419,41 +413,42 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
         <v>6.83</v>
@@ -462,7 +457,7 @@
         <v>6.8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2">
         <v>6.71</v>
@@ -470,10 +465,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>23.34</v>
@@ -490,10 +485,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>19.350000000000001</v>
@@ -510,10 +505,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
         <v>3.84</v>
@@ -529,24 +524,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2">
-        <v>19.38</v>
-      </c>
-      <c r="D6" s="2">
-        <v>19.579999999999998</v>
-      </c>
-      <c r="E6" s="2">
-        <v>19.350000000000001</v>
-      </c>
-      <c r="F6" s="2">
-        <v>19.690000000000001</v>
-      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>